<commit_message>
[SMD-746]: cell indexes for cross validation failures
..

..
</commit_message>
<xml_diff>
--- a/tests/integration_tests/mock_pf_returns/PF_Round_1_Cross_Table_Validation_Failures.xlsx
+++ b/tests/integration_tests/mock_pf_returns/PF_Round_1_Cross_Table_Validation_Failures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PearceJ\stash\funding-service-design-post-award-data-store\tests\integration_tests\mock_pf_returns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CED9DD-8DFF-4641-8A61-97788A2CDB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07C1649-3385-4540-8E5A-16BE83B5CB68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="661" firstSheet="4" activeTab="10" xr2:uid="{F1A93CD4-AFD6-463B-B066-EB4D40A0C607}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="661" firstSheet="4" activeTab="7" xr2:uid="{F1A93CD4-AFD6-463B-B066-EB4D40A0C607}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="13" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2903" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2903" uniqueCount="1125">
   <si>
     <t>Reporting Round</t>
   </si>
@@ -3785,6 +3785,9 @@
   </si>
   <si>
     <t>Enhancing sub-regional and regional connectivity</t>
+  </si>
+  <si>
+    <t>Not allowed</t>
   </si>
 </sst>
 </file>
@@ -7927,7 +7930,7 @@
   </sheetPr>
   <dimension ref="A1:J177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="B180" sqref="B180"/>
     </sheetView>
   </sheetViews>
@@ -37690,8 +37693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD05DD0-7124-4A36-99BE-80113683F5E3}">
   <dimension ref="A2:AF90"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P74" sqref="P74:Q74"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -40461,7 +40464,7 @@
       </c>
       <c r="D70" s="379"/>
       <c r="E70" s="359" t="s">
-        <v>302</v>
+        <v>1124</v>
       </c>
       <c r="F70" s="359"/>
       <c r="G70" s="379" t="s">

</xml_diff>

<commit_message>
[SMD-746]: cell indexes for cross validation failures (#527)
</commit_message>
<xml_diff>
--- a/tests/integration_tests/mock_pf_returns/PF_Round_1_Cross_Table_Validation_Failures.xlsx
+++ b/tests/integration_tests/mock_pf_returns/PF_Round_1_Cross_Table_Validation_Failures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PearceJ\stash\funding-service-design-post-award-data-store\tests\integration_tests\mock_pf_returns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CED9DD-8DFF-4641-8A61-97788A2CDB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07C1649-3385-4540-8E5A-16BE83B5CB68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="661" firstSheet="4" activeTab="10" xr2:uid="{F1A93CD4-AFD6-463B-B066-EB4D40A0C607}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="661" firstSheet="4" activeTab="7" xr2:uid="{F1A93CD4-AFD6-463B-B066-EB4D40A0C607}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="13" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2903" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2903" uniqueCount="1125">
   <si>
     <t>Reporting Round</t>
   </si>
@@ -3785,6 +3785,9 @@
   </si>
   <si>
     <t>Enhancing sub-regional and regional connectivity</t>
+  </si>
+  <si>
+    <t>Not allowed</t>
   </si>
 </sst>
 </file>
@@ -7927,7 +7930,7 @@
   </sheetPr>
   <dimension ref="A1:J177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="B180" sqref="B180"/>
     </sheetView>
   </sheetViews>
@@ -37690,8 +37693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD05DD0-7124-4A36-99BE-80113683F5E3}">
   <dimension ref="A2:AF90"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P74" sqref="P74:Q74"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -40461,7 +40464,7 @@
       </c>
       <c r="D70" s="379"/>
       <c r="E70" s="359" t="s">
-        <v>302</v>
+        <v>1124</v>
       </c>
       <c r="F70" s="359"/>
       <c r="G70" s="379" t="s">

</xml_diff>